<commit_message>
added CertTest and moved wind data inputs to CertTest/data folder added lidar module (involved adding some additional possible inputs and moving a bunch of CalcOutput into a subroutine in InflowWind_Subs.f90). updated types files modified makefile so it runs on Windows. Need to check if all my changes also work on Mac! added some destroy routines based on results from Intel Inspector commented out HAWCWind lines in InflowWind.txt
git-svn-id: https://windsvn2.nrel.gov/InflowWind/branches/modularization2@165 96535b8f-fecd-4773-a067-ac893715d582
</commit_message>
<xml_diff>
--- a/OutListParameters.xlsx
+++ b/OutListParameters.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="1200" windowWidth="32560" windowHeight="19040" activeTab="1"/>
+    <workbookView xWindow="2196" yWindow="1200" windowWidth="20844" windowHeight="9924" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
     <sheet name="InflowWind" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="105">
   <si>
     <t>Category</t>
   </si>
@@ -285,6 +285,57 @@
   </si>
   <si>
     <t>Z component of wind at user selected wind point 9</t>
+  </si>
+  <si>
+    <t>WindMeas1</t>
+  </si>
+  <si>
+    <t>WindMeas2</t>
+  </si>
+  <si>
+    <t>WindMeas3</t>
+  </si>
+  <si>
+    <t>WindMeas4</t>
+  </si>
+  <si>
+    <t>WindMeas5</t>
+  </si>
+  <si>
+    <t>Wind measurement at sensor 1</t>
+  </si>
+  <si>
+    <t>Wind measurement at sensor 2</t>
+  </si>
+  <si>
+    <t>Wind measurement at sensor 3</t>
+  </si>
+  <si>
+    <t>Wind measurement at sensor 4</t>
+  </si>
+  <si>
+    <t>Wind measurement at sensor 5</t>
+  </si>
+  <si>
+    <t>Defined by sensor</t>
+  </si>
+  <si>
+    <t>Wind Sensor Measurements</t>
+  </si>
+  <si>
+    <t>p%lidar%SensorType == SensorType_None</t>
+  </si>
+  <si>
+    <t>p%lidar%NumPulseGate &lt; 2</t>
+  </si>
+  <si>
+    <t>p%lidar%NumPulseGate &lt; 3</t>
+  </si>
+  <si>
+    <t>p%lidar%NumPulseGate &lt; 4</t>
+  </si>
+  <si>
+    <t>p%lidar%NumPulseGate &lt; 5</t>
   </si>
 </sst>
 </file>
@@ -754,47 +805,47 @@
   <dimension ref="A3:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="D8">
         <f>COUNTA(InflowWind!B2:B1333)</f>
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>18</v>
       </c>
@@ -802,7 +853,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -810,7 +861,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -818,7 +869,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -826,7 +877,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -834,7 +885,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -842,7 +893,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -850,7 +901,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -875,24 +926,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -915,7 +966,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -923,7 +974,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>34</v>
       </c>
@@ -937,7 +988,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>35</v>
       </c>
@@ -951,7 +1002,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
@@ -965,7 +1016,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
         <v>40</v>
       </c>
@@ -979,7 +1030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>41</v>
       </c>
@@ -993,7 +1044,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>42</v>
       </c>
@@ -1007,7 +1058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="9" t="s">
         <v>46</v>
       </c>
@@ -1021,7 +1072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>47</v>
       </c>
@@ -1035,7 +1086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>48</v>
       </c>
@@ -1049,7 +1100,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="9" t="s">
         <v>52</v>
       </c>
@@ -1063,7 +1114,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>53</v>
       </c>
@@ -1077,7 +1128,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>54</v>
       </c>
@@ -1091,7 +1142,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="9" t="s">
         <v>58</v>
       </c>
@@ -1105,7 +1156,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>59</v>
       </c>
@@ -1119,7 +1170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>60</v>
       </c>
@@ -1133,7 +1184,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B18" s="9" t="s">
         <v>64</v>
       </c>
@@ -1147,7 +1198,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
         <v>65</v>
       </c>
@@ -1161,7 +1212,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>66</v>
       </c>
@@ -1175,7 +1226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="s">
         <v>70</v>
       </c>
@@ -1189,7 +1240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>71</v>
       </c>
@@ -1203,7 +1254,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
         <v>72</v>
       </c>
@@ -1217,7 +1268,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="s">
         <v>76</v>
       </c>
@@ -1231,7 +1282,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
         <v>77</v>
       </c>
@@ -1245,7 +1296,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
         <v>78</v>
       </c>
@@ -1259,7 +1310,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B27" s="9" t="s">
         <v>82</v>
       </c>
@@ -1273,7 +1324,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
         <v>83</v>
       </c>
@@ -1287,7 +1338,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
         <v>84</v>
       </c>
@@ -1301,17 +1352,98 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="2:6">
-      <c r="E30" s="6"/>
-      <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="2:6">
-      <c r="E31" s="6"/>
-      <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="2:6">
-      <c r="E32" s="6"/>
-      <c r="F32" s="5"/>
+    <row r="30" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B32" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" t="s">
+        <v>104</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1330,7 +1462,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>